<commit_message>
updated new size pngs
</commit_message>
<xml_diff>
--- a/Q3/Q3Table SPXput.xlsx
+++ b/Q3/Q3Table SPXput.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GithubQUB\FIN9007\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GithubQUB\FIN9007\Q3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F4AB33-5E2B-47E7-A728-D6CF6EB16165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35CD3299-9422-4822-8515-0AD9D45417FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23172" yWindow="-132" windowWidth="23304" windowHeight="12504" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="4" r:id="rId1"/>
@@ -79,10 +79,10 @@
     <t>Sample of Tree resultsof all expiryDates, Selected strike=4000</t>
   </si>
   <si>
-    <t>Descriptive Statistics</t>
+    <t>SD</t>
   </si>
   <si>
-    <t>SD</t>
+    <t xml:space="preserve">Descriptive Statistics SPX put </t>
   </si>
 </sst>
 </file>
@@ -730,10 +730,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1092,7 +1092,7 @@
   <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1164,14 +1164,14 @@
       <c r="G3" s="12">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="I3" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
+      <c r="I3" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="11">
@@ -1294,20 +1294,20 @@
       <c r="G7" s="12">
         <v>1.1499999999999999</v>
       </c>
-      <c r="I7" s="17" t="s">
-        <v>16</v>
+      <c r="I7" s="16" t="s">
+        <v>15</v>
       </c>
       <c r="J7">
         <v>198.54080938177466</v>
       </c>
-      <c r="K7" s="17" t="s">
-        <v>16</v>
+      <c r="K7" s="16" t="s">
+        <v>15</v>
       </c>
       <c r="L7" s="1">
         <v>194.86160475352085</v>
       </c>
-      <c r="M7" s="17" t="s">
-        <v>16</v>
+      <c r="M7" s="16" t="s">
+        <v>15</v>
       </c>
       <c r="N7" s="1">
         <v>52.024105131923328</v>

</xml_diff>